<commit_message>
minor dd lower buff
</commit_message>
<xml_diff>
--- a/changes/m4-lowers.xlsx
+++ b/changes/m4-lowers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BDD364F-0F40-4871-B2E0-7471EF13126B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC8C9A1-5A94-46D4-81A2-3EC8D740EBF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>new</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>Aeroknox AX // 15 Lower Receiver</t>
+  </si>
+  <si>
+    <t>daniel_defense_m4_carbine_lower_receiver</t>
+  </si>
+  <si>
+    <t>Daniel Defense M4 Carbine Lower Receiver</t>
   </si>
 </sst>
 </file>
@@ -998,10 +1004,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1081,220 +1087,202 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
       <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>0.33</v>
+      </c>
+      <c r="M4">
+        <v>1000</v>
+      </c>
+      <c r="N4">
+        <f t="shared" ref="N4:N19" si="0">C4-D4*20-E4*0.8-F4*0.6</f>
+        <v>-2.6000000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>34</v>
       </c>
-      <c r="C4">
-        <f>C3+C16+C11</f>
-        <v>4</v>
-      </c>
-      <c r="D4">
-        <f t="shared" ref="D4:F4" si="0">D3+D16+D11</f>
-        <v>0.39</v>
-      </c>
-      <c r="E4">
+      <c r="C5">
+        <f>C3+C18</f>
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:F5" si="1">D3+D18</f>
+        <v>0.32</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>-4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:E6" si="2">C4+C18</f>
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="2"/>
+        <v>0.35000000000000003</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f>F4+F18</f>
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>-1.0000000000000009</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>0.42</v>
+      </c>
+      <c r="E7">
+        <v>-2</v>
+      </c>
+      <c r="F7">
+        <v>-3</v>
+      </c>
+      <c r="M7">
+        <v>4000</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999956</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>0.35</v>
+      </c>
+      <c r="E8">
+        <v>-2</v>
+      </c>
+      <c r="F8">
+        <v>-1</v>
+      </c>
+      <c r="M8">
+        <v>2000</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>0.20000000000000007</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>0.25</v>
+      </c>
+      <c r="E9">
+        <v>-1</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>1500</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>0.23</v>
+      </c>
+      <c r="E10">
+        <v>-6</v>
+      </c>
+      <c r="F10">
+        <v>12</v>
+      </c>
+      <c r="M10">
+        <v>3000</v>
+      </c>
+      <c r="N10">
+        <f>C10-D10*20-E10*0.8-F10*0.6</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F4">
-        <f t="shared" si="0"/>
-        <v>-2</v>
-      </c>
-      <c r="N4">
-        <f t="shared" ref="N4:N17" si="1">C4-D4*20-E4*0.8-F4*0.6</f>
-        <v>-2.6000000000000005</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5">
-        <v>8</v>
-      </c>
-      <c r="D5">
-        <v>0.23</v>
-      </c>
-      <c r="E5">
-        <v>-6</v>
-      </c>
-      <c r="F5">
-        <v>12</v>
-      </c>
-      <c r="M5">
-        <v>3000</v>
-      </c>
-      <c r="N5">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6">
-        <v>6</v>
-      </c>
-      <c r="D6">
-        <v>0.42</v>
-      </c>
-      <c r="E6">
-        <v>-2</v>
-      </c>
-      <c r="F6">
-        <v>-4</v>
-      </c>
-      <c r="M6">
-        <v>4000</v>
-      </c>
-      <c r="N6">
-        <f t="shared" si="1"/>
-        <v>1.5999999999999996</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7">
-        <v>5</v>
-      </c>
-      <c r="D7">
-        <v>0.35</v>
-      </c>
-      <c r="E7">
-        <v>-2</v>
-      </c>
-      <c r="F7">
-        <v>-1</v>
-      </c>
-      <c r="M7">
-        <v>2000</v>
-      </c>
-      <c r="N7">
-        <f t="shared" si="1"/>
-        <v>0.20000000000000007</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-      <c r="D8">
-        <v>0.25</v>
-      </c>
-      <c r="E8">
-        <v>-1</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>1500</v>
-      </c>
-      <c r="N8">
-        <f t="shared" si="1"/>
-        <v>-1.2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="N9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="1">
-        <v>3</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0.13</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1">
-        <v>750</v>
-      </c>
-      <c r="N10">
-        <f t="shared" si="1"/>
-        <v>0.39999999999999991</v>
-      </c>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="1">
-        <v>2</v>
-      </c>
-      <c r="D11" s="1">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1">
-        <v>-2</v>
-      </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1">
-        <v>500</v>
-      </c>
-      <c r="N11">
-        <f t="shared" si="1"/>
-        <v>1.7999999999999998</v>
-      </c>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C12" s="1">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="D12" s="1">
-        <v>0.05</v>
+        <v>0.13</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -1305,84 +1293,108 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1">
-        <v>250</v>
+        <v>750</v>
       </c>
       <c r="N12">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
+        <f t="shared" si="0"/>
+        <v>0.39999999999999991</v>
       </c>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E13" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>-1</v>
+      </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
+      <c r="M13" s="1">
+        <v>500</v>
+      </c>
       <c r="N13">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.99999999999999989</v>
       </c>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14">
+      <c r="A14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="1">
         <v>2</v>
       </c>
-      <c r="D14">
-        <v>0.02</v>
-      </c>
-      <c r="M14">
-        <v>200</v>
+      <c r="D14" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1">
+        <v>250</v>
       </c>
       <c r="N14">
-        <f t="shared" si="1"/>
-        <v>1.6</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15">
-        <v>2.5</v>
-      </c>
-      <c r="D15">
-        <v>0.05</v>
-      </c>
-      <c r="M15">
-        <v>200</v>
-      </c>
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
       <c r="N15">
-        <f t="shared" si="1"/>
-        <v>1.5</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -1391,31 +1403,73 @@
         <v>0.02</v>
       </c>
       <c r="M16">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="N16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.6</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17">
+        <v>2.5</v>
+      </c>
+      <c r="D17">
+        <v>0.05</v>
+      </c>
+      <c r="M17">
+        <v>200</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>0.02</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="0"/>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>29</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B19" t="s">
         <v>30</v>
       </c>
-      <c r="C17">
+      <c r="C19">
         <v>3</v>
       </c>
-      <c r="D17">
+      <c r="D19">
         <v>0.08</v>
       </c>
-      <c r="M17">
+      <c r="M19">
         <v>400</v>
       </c>
-      <c r="N17">
-        <f t="shared" si="1"/>
+      <c r="N19">
+        <f t="shared" si="0"/>
         <v>1.4</v>
       </c>
     </row>

</xml_diff>